<commit_message>
26 Nisan 2020 verileri eklendi
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\python\workspace\covid19-tr-analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\github\covid19-turkey\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0C1F06C-49E3-4E54-B6F9-9F207D813BA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{289F754C-3EED-499A-B7BA-6E10323D63AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -605,8 +605,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CE9BAF82-BB88-4AAB-90E2-12667B1414BA}" name="Table3" displayName="Table3" ref="A1:E45" totalsRowShown="0">
-  <autoFilter ref="A1:E45" xr:uid="{EFB3D828-C984-40FA-93EF-F15786C73A15}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CE9BAF82-BB88-4AAB-90E2-12667B1414BA}" name="Table3" displayName="Table3" ref="A1:E46" totalsRowShown="0">
+  <autoFilter ref="A1:E46" xr:uid="{EFB3D828-C984-40FA-93EF-F15786C73A15}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00C2DB9E-C1C1-40DE-8B3F-FA6C7D48E039}" name="date" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{35622F43-3A84-488A-949F-E03870DE3E7F}" name="test" dataDxfId="3"/>
@@ -915,10 +915,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1625,6 +1625,23 @@
         <v>3845</v>
       </c>
     </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>43947</v>
+      </c>
+      <c r="B46" s="2">
+        <v>30177</v>
+      </c>
+      <c r="C46" s="2">
+        <v>2357</v>
+      </c>
+      <c r="D46" s="2">
+        <v>99</v>
+      </c>
+      <c r="E46" s="2">
+        <v>3558</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
27 Nisan 2020 verileri eklendi
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\github\covid19-turkey\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{289F754C-3EED-499A-B7BA-6E10323D63AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E4A8266-94CA-4B63-90B0-6FE8DBF5B967}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -605,8 +605,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CE9BAF82-BB88-4AAB-90E2-12667B1414BA}" name="Table3" displayName="Table3" ref="A1:E46" totalsRowShown="0">
-  <autoFilter ref="A1:E46" xr:uid="{EFB3D828-C984-40FA-93EF-F15786C73A15}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CE9BAF82-BB88-4AAB-90E2-12667B1414BA}" name="Table3" displayName="Table3" ref="A1:E47" totalsRowShown="0">
+  <autoFilter ref="A1:E47" xr:uid="{EFB3D828-C984-40FA-93EF-F15786C73A15}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00C2DB9E-C1C1-40DE-8B3F-FA6C7D48E039}" name="date" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{35622F43-3A84-488A-949F-E03870DE3E7F}" name="test" dataDxfId="3"/>
@@ -915,10 +915,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1642,6 +1642,23 @@
         <v>3558</v>
       </c>
     </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>43948</v>
+      </c>
+      <c r="B47" s="2">
+        <v>20143</v>
+      </c>
+      <c r="C47" s="2">
+        <v>2131</v>
+      </c>
+      <c r="D47" s="2">
+        <v>95</v>
+      </c>
+      <c r="E47" s="2">
+        <v>4651</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
28 Nisan ve 29 Nisan 2020 verilerileri eklendi
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\github\covid19-turkey\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E4A8266-94CA-4B63-90B0-6FE8DBF5B967}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{351474FB-C77A-49F1-9F76-A09195DD8F4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -605,8 +605,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CE9BAF82-BB88-4AAB-90E2-12667B1414BA}" name="Table3" displayName="Table3" ref="A1:E47" totalsRowShown="0">
-  <autoFilter ref="A1:E47" xr:uid="{EFB3D828-C984-40FA-93EF-F15786C73A15}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CE9BAF82-BB88-4AAB-90E2-12667B1414BA}" name="Table3" displayName="Table3" ref="A1:E49" totalsRowShown="0">
+  <autoFilter ref="A1:E49" xr:uid="{EFB3D828-C984-40FA-93EF-F15786C73A15}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00C2DB9E-C1C1-40DE-8B3F-FA6C7D48E039}" name="date" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{35622F43-3A84-488A-949F-E03870DE3E7F}" name="test" dataDxfId="3"/>
@@ -915,10 +915,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1659,6 +1659,40 @@
         <v>4651</v>
       </c>
     </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>43949</v>
+      </c>
+      <c r="B48" s="2">
+        <v>29230</v>
+      </c>
+      <c r="C48" s="2">
+        <v>2392</v>
+      </c>
+      <c r="D48" s="2">
+        <v>92</v>
+      </c>
+      <c r="E48" s="2">
+        <v>5018</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>43950</v>
+      </c>
+      <c r="B49" s="2">
+        <v>43498</v>
+      </c>
+      <c r="C49" s="2">
+        <v>2936</v>
+      </c>
+      <c r="D49" s="2">
+        <v>89</v>
+      </c>
+      <c r="E49" s="2">
+        <v>5231</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
30 Nisan 2020 verileri eklendi
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\github\covid19-turkey\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{351474FB-C77A-49F1-9F76-A09195DD8F4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEFF6424-0CB0-4E81-8141-8576D000AECA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -605,8 +605,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CE9BAF82-BB88-4AAB-90E2-12667B1414BA}" name="Table3" displayName="Table3" ref="A1:E49" totalsRowShown="0">
-  <autoFilter ref="A1:E49" xr:uid="{EFB3D828-C984-40FA-93EF-F15786C73A15}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CE9BAF82-BB88-4AAB-90E2-12667B1414BA}" name="Table3" displayName="Table3" ref="A1:E50" totalsRowShown="0">
+  <autoFilter ref="A1:E50" xr:uid="{EFB3D828-C984-40FA-93EF-F15786C73A15}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00C2DB9E-C1C1-40DE-8B3F-FA6C7D48E039}" name="date" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{35622F43-3A84-488A-949F-E03870DE3E7F}" name="test" dataDxfId="3"/>
@@ -915,10 +915,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1693,6 +1693,23 @@
         <v>5231</v>
       </c>
     </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>43951</v>
+      </c>
+      <c r="B50" s="2">
+        <v>42004</v>
+      </c>
+      <c r="C50" s="2">
+        <v>2615</v>
+      </c>
+      <c r="D50" s="2">
+        <v>93</v>
+      </c>
+      <c r="E50" s="2">
+        <v>4846</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
1 Mayıs 2020 verileri eklendi
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,14 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\github\covid19-turkey\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEFF6424-0CB0-4E81-8141-8576D000AECA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E52B915-F471-4B56-93A9-3D9C57C20D34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -605,8 +615,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CE9BAF82-BB88-4AAB-90E2-12667B1414BA}" name="Table3" displayName="Table3" ref="A1:E50" totalsRowShown="0">
-  <autoFilter ref="A1:E50" xr:uid="{EFB3D828-C984-40FA-93EF-F15786C73A15}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CE9BAF82-BB88-4AAB-90E2-12667B1414BA}" name="Table3" displayName="Table3" ref="A1:E51" totalsRowShown="0">
+  <autoFilter ref="A1:E51" xr:uid="{EFB3D828-C984-40FA-93EF-F15786C73A15}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00C2DB9E-C1C1-40DE-8B3F-FA6C7D48E039}" name="date" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{35622F43-3A84-488A-949F-E03870DE3E7F}" name="test" dataDxfId="3"/>
@@ -915,10 +925,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1710,6 +1720,23 @@
         <v>4846</v>
       </c>
     </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>43952</v>
+      </c>
+      <c r="B51" s="2">
+        <v>41.430999999999997</v>
+      </c>
+      <c r="C51" s="2">
+        <v>2.1880000000000002</v>
+      </c>
+      <c r="D51" s="2">
+        <v>84</v>
+      </c>
+      <c r="E51" s="2">
+        <v>4922</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
2 Mayıs 2020 verileri eklendi
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\github\covid19-turkey\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E52B915-F471-4B56-93A9-3D9C57C20D34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8427C6EE-F589-43E8-A4CF-1960B2781D15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -615,8 +615,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CE9BAF82-BB88-4AAB-90E2-12667B1414BA}" name="Table3" displayName="Table3" ref="A1:E51" totalsRowShown="0">
-  <autoFilter ref="A1:E51" xr:uid="{EFB3D828-C984-40FA-93EF-F15786C73A15}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CE9BAF82-BB88-4AAB-90E2-12667B1414BA}" name="Table3" displayName="Table3" ref="A1:E52" totalsRowShown="0">
+  <autoFilter ref="A1:E52" xr:uid="{EFB3D828-C984-40FA-93EF-F15786C73A15}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00C2DB9E-C1C1-40DE-8B3F-FA6C7D48E039}" name="date" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{35622F43-3A84-488A-949F-E03870DE3E7F}" name="test" dataDxfId="3"/>
@@ -925,10 +925,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1737,6 +1737,23 @@
         <v>4922</v>
       </c>
     </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>43953</v>
+      </c>
+      <c r="B52" s="2">
+        <v>36318</v>
+      </c>
+      <c r="C52" s="2">
+        <v>1983</v>
+      </c>
+      <c r="D52" s="2">
+        <v>78</v>
+      </c>
+      <c r="E52" s="2">
+        <v>4451</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
3 Mayıs 2020 verileri eklendi
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\github\covid19-turkey\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8427C6EE-F589-43E8-A4CF-1960B2781D15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399CFDF8-8AA7-4B4E-9BFE-FEB3E05A4352}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -615,8 +615,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CE9BAF82-BB88-4AAB-90E2-12667B1414BA}" name="Table3" displayName="Table3" ref="A1:E52" totalsRowShown="0">
-  <autoFilter ref="A1:E52" xr:uid="{EFB3D828-C984-40FA-93EF-F15786C73A15}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CE9BAF82-BB88-4AAB-90E2-12667B1414BA}" name="Table3" displayName="Table3" ref="A1:E53" totalsRowShown="0">
+  <autoFilter ref="A1:E53" xr:uid="{EFB3D828-C984-40FA-93EF-F15786C73A15}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00C2DB9E-C1C1-40DE-8B3F-FA6C7D48E039}" name="date" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{35622F43-3A84-488A-949F-E03870DE3E7F}" name="test" dataDxfId="3"/>
@@ -925,10 +925,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1754,6 +1754,23 @@
         <v>4451</v>
       </c>
     </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>43954</v>
+      </c>
+      <c r="B53" s="2">
+        <v>24001</v>
+      </c>
+      <c r="C53" s="2">
+        <v>1670</v>
+      </c>
+      <c r="D53" s="2">
+        <v>61</v>
+      </c>
+      <c r="E53" s="2">
+        <v>4892</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
4 Mayıs 2020 verileri eklendi
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\github\covid19-turkey\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399CFDF8-8AA7-4B4E-9BFE-FEB3E05A4352}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E5BBF4-8AF6-4548-A42D-A38BA98059BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -615,8 +615,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CE9BAF82-BB88-4AAB-90E2-12667B1414BA}" name="Table3" displayName="Table3" ref="A1:E53" totalsRowShown="0">
-  <autoFilter ref="A1:E53" xr:uid="{EFB3D828-C984-40FA-93EF-F15786C73A15}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CE9BAF82-BB88-4AAB-90E2-12667B1414BA}" name="Table3" displayName="Table3" ref="A1:E54" totalsRowShown="0">
+  <autoFilter ref="A1:E54" xr:uid="{EFB3D828-C984-40FA-93EF-F15786C73A15}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00C2DB9E-C1C1-40DE-8B3F-FA6C7D48E039}" name="date" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{35622F43-3A84-488A-949F-E03870DE3E7F}" name="test" dataDxfId="3"/>
@@ -925,7 +925,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
       <selection activeCell="E53" sqref="E53"/>
@@ -1771,6 +1771,23 @@
         <v>4892</v>
       </c>
     </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>43955</v>
+      </c>
+      <c r="B54" s="2">
+        <v>35771</v>
+      </c>
+      <c r="C54" s="2">
+        <v>1614</v>
+      </c>
+      <c r="D54" s="2">
+        <v>64</v>
+      </c>
+      <c r="E54" s="2">
+        <v>5015</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
5 Mayıs 2020 verileri eklendi
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\github\covid19-turkey\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E5BBF4-8AF6-4548-A42D-A38BA98059BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BDF9F7-7D40-4F13-84C2-707233C70A58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -615,8 +615,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CE9BAF82-BB88-4AAB-90E2-12667B1414BA}" name="Table3" displayName="Table3" ref="A1:E54" totalsRowShown="0">
-  <autoFilter ref="A1:E54" xr:uid="{EFB3D828-C984-40FA-93EF-F15786C73A15}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CE9BAF82-BB88-4AAB-90E2-12667B1414BA}" name="Table3" displayName="Table3" ref="A1:E55" totalsRowShown="0">
+  <autoFilter ref="A1:E55" xr:uid="{EFB3D828-C984-40FA-93EF-F15786C73A15}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00C2DB9E-C1C1-40DE-8B3F-FA6C7D48E039}" name="date" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{35622F43-3A84-488A-949F-E03870DE3E7F}" name="test" dataDxfId="3"/>
@@ -925,10 +925,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E54"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+      <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1788,6 +1788,23 @@
         <v>5015</v>
       </c>
     </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>43956</v>
+      </c>
+      <c r="B55" s="2">
+        <v>33283</v>
+      </c>
+      <c r="C55" s="2">
+        <v>1832</v>
+      </c>
+      <c r="D55" s="2">
+        <v>59</v>
+      </c>
+      <c r="E55" s="2">
+        <v>5119</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
6 Mayıs 2020 verileri eklendi
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\github\covid19-turkey\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mehmet\Desktop\github\covid19-turkey\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BDF9F7-7D40-4F13-84C2-707233C70A58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -50,7 +49,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -541,48 +540,48 @@
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="%20 - Vurgu1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="%20 - Vurgu2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="%20 - Vurgu3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="%20 - Vurgu4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="%20 - Vurgu5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="%20 - Vurgu6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="%40 - Vurgu1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="%40 - Vurgu2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="%40 - Vurgu3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="%40 - Vurgu4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="%40 - Vurgu5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="%40 - Vurgu6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="%60 - Vurgu1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="%60 - Vurgu2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="%60 - Vurgu3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="%60 - Vurgu4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="%60 - Vurgu5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="%60 - Vurgu6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Açıklama Metni" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Ana Başlık" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Bağlı Hücre" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Başlık 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Başlık 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Başlık 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Başlık 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Çıkış" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Giriş" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Hesaplama" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="İşaretli Hücre" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="İyi" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Kötü" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Not" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Nötr" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Toplam" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Uyarı Metni" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Vurgu1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Vurgu2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Vurgu3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Vurgu4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Vurgu5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Vurgu6" xfId="38" builtinId="49" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
@@ -615,14 +614,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CE9BAF82-BB88-4AAB-90E2-12667B1414BA}" name="Table3" displayName="Table3" ref="A1:E55" totalsRowShown="0">
-  <autoFilter ref="A1:E55" xr:uid="{EFB3D828-C984-40FA-93EF-F15786C73A15}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:E56" totalsRowShown="0">
+  <autoFilter ref="A1:E56"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00C2DB9E-C1C1-40DE-8B3F-FA6C7D48E039}" name="date" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{35622F43-3A84-488A-949F-E03870DE3E7F}" name="test" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{46AD1946-9BE0-4A5D-8A56-01CAAD008B49}" name="case" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{65373A0C-DF63-4913-AF0F-EDD51E8D81C6}" name="death" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{38124B9B-1958-4A9D-9B29-754B01CFF080}" name="recovered" dataDxfId="0"/>
+    <tableColumn id="1" name="date" dataDxfId="4"/>
+    <tableColumn id="2" name="test" dataDxfId="3"/>
+    <tableColumn id="3" name="case" dataDxfId="2"/>
+    <tableColumn id="4" name="death" dataDxfId="1"/>
+    <tableColumn id="5" name="recovered" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -924,11 +923,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1805,6 +1804,23 @@
         <v>5119</v>
       </c>
     </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>43957</v>
+      </c>
+      <c r="B56" s="2">
+        <v>30303</v>
+      </c>
+      <c r="C56" s="2">
+        <v>2253</v>
+      </c>
+      <c r="D56" s="2">
+        <v>64</v>
+      </c>
+      <c r="E56" s="2">
+        <v>4917</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
7 Mayıs 2020 verileri eklendi
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -614,8 +614,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:E56" totalsRowShown="0">
-  <autoFilter ref="A1:E56"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:E57" totalsRowShown="0">
+  <autoFilter ref="A1:E57"/>
   <tableColumns count="5">
     <tableColumn id="1" name="date" dataDxfId="4"/>
     <tableColumn id="2" name="test" dataDxfId="3"/>
@@ -924,10 +924,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1821,6 +1821,23 @@
         <v>4917</v>
       </c>
     </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>43958</v>
+      </c>
+      <c r="B57" s="2">
+        <v>30395</v>
+      </c>
+      <c r="C57" s="2">
+        <v>1977</v>
+      </c>
+      <c r="D57" s="2">
+        <v>57</v>
+      </c>
+      <c r="E57" s="2">
+        <v>4782</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
8 Mayıs 2020 verileri eklendi
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -614,8 +614,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:E57" totalsRowShown="0">
-  <autoFilter ref="A1:E57"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:E58" totalsRowShown="0">
+  <autoFilter ref="A1:E58"/>
   <tableColumns count="5">
     <tableColumn id="1" name="date" dataDxfId="4"/>
     <tableColumn id="2" name="test" dataDxfId="3"/>
@@ -924,10 +924,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E57"/>
+  <dimension ref="A1:E58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1838,6 +1838,23 @@
         <v>4782</v>
       </c>
     </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>43959</v>
+      </c>
+      <c r="B58" s="2">
+        <v>33687</v>
+      </c>
+      <c r="C58" s="2">
+        <v>1848</v>
+      </c>
+      <c r="D58" s="2">
+        <v>48</v>
+      </c>
+      <c r="E58" s="2">
+        <v>3412</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
9 Mayıs 2020 verileri eklendi
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -530,12 +530,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -614,8 +617,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:E58" totalsRowShown="0">
-  <autoFilter ref="A1:E58"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:E59" totalsRowShown="0">
+  <autoFilter ref="A1:E59"/>
   <tableColumns count="5">
     <tableColumn id="1" name="date" dataDxfId="4"/>
     <tableColumn id="2" name="test" dataDxfId="3"/>
@@ -924,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:E59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1855,6 +1858,23 @@
         <v>3412</v>
       </c>
     </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>43960</v>
+      </c>
+      <c r="B59" s="3">
+        <v>35605</v>
+      </c>
+      <c r="C59" s="2">
+        <v>1546</v>
+      </c>
+      <c r="D59" s="2">
+        <v>50</v>
+      </c>
+      <c r="E59" s="2">
+        <v>3084</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
10 Mayıs 2020 verileri eklendi
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -617,8 +617,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:E59" totalsRowShown="0">
-  <autoFilter ref="A1:E59"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:E60" totalsRowShown="0">
+  <autoFilter ref="A1:E60"/>
   <tableColumns count="5">
     <tableColumn id="1" name="date" dataDxfId="4"/>
     <tableColumn id="2" name="test" dataDxfId="3"/>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E59"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1875,6 +1875,23 @@
         <v>3084</v>
       </c>
     </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>43961</v>
+      </c>
+      <c r="B60" s="2">
+        <v>36187</v>
+      </c>
+      <c r="C60" s="2">
+        <v>1542</v>
+      </c>
+      <c r="D60" s="2">
+        <v>47</v>
+      </c>
+      <c r="E60" s="2">
+        <v>3211</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
11 Mayıs 2020 verileri eklendi
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1,30 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mehmet\Desktop\github\covid19-turkey\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\github\covid19-turkey\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74AFA46B-1C60-469E-B66F-A422059B5065}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -49,7 +40,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -543,48 +534,48 @@
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="%20 - Vurgu1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="%20 - Vurgu2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="%20 - Vurgu3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="%20 - Vurgu4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="%20 - Vurgu5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="%20 - Vurgu6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="%40 - Vurgu1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="%40 - Vurgu2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="%40 - Vurgu3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="%40 - Vurgu4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="%40 - Vurgu5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="%40 - Vurgu6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="%60 - Vurgu1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="%60 - Vurgu2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="%60 - Vurgu3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="%60 - Vurgu4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="%60 - Vurgu5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="%60 - Vurgu6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Açıklama Metni" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Ana Başlık" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Bağlı Hücre" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Başlık 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Başlık 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Başlık 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Başlık 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Çıkış" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Giriş" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Hesaplama" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="İşaretli Hücre" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="İyi" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Kötü" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Not" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Nötr" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Toplam" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Uyarı Metni" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Vurgu1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Vurgu2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Vurgu3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Vurgu4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Vurgu5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Vurgu6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
@@ -617,14 +608,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:E60" totalsRowShown="0">
-  <autoFilter ref="A1:E60"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:E61" totalsRowShown="0">
+  <autoFilter ref="A1:E61" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="date" dataDxfId="4"/>
-    <tableColumn id="2" name="test" dataDxfId="3"/>
-    <tableColumn id="3" name="case" dataDxfId="2"/>
-    <tableColumn id="4" name="death" dataDxfId="1"/>
-    <tableColumn id="5" name="recovered" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="date" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="test" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="case" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="death" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="recovered" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -926,11 +917,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E60"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+      <selection activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1892,6 +1883,23 @@
         <v>3211</v>
       </c>
     </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>43962</v>
+      </c>
+      <c r="B61" s="2">
+        <v>32722</v>
+      </c>
+      <c r="C61" s="2">
+        <v>1114</v>
+      </c>
+      <c r="D61" s="2">
+        <v>55</v>
+      </c>
+      <c r="E61" s="2">
+        <v>3089</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
12 Mayıs 2020 verileri eklendi
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\github\covid19-turkey\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74AFA46B-1C60-469E-B66F-A422059B5065}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D824E1A3-CA3F-42C5-A213-105CDE33CFBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -608,8 +608,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:E61" totalsRowShown="0">
-  <autoFilter ref="A1:E61" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:E62" totalsRowShown="0">
+  <autoFilter ref="A1:E62" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="date" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="test" dataDxfId="3"/>
@@ -918,10 +918,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="E60" sqref="E60"/>
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1900,6 +1900,23 @@
         <v>3089</v>
       </c>
     </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>43963</v>
+      </c>
+      <c r="B62" s="2">
+        <v>37351</v>
+      </c>
+      <c r="C62" s="2">
+        <v>1704</v>
+      </c>
+      <c r="D62" s="2">
+        <v>53</v>
+      </c>
+      <c r="E62" s="2">
+        <v>3109</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
13 Mayıs 2020 verileri eklendi
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\github\covid19-turkey\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D824E1A3-CA3F-42C5-A213-105CDE33CFBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1572F037-7A9E-4F37-AAD2-46425ABB51A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -608,8 +608,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:E62" totalsRowShown="0">
-  <autoFilter ref="A1:E62" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:E63" totalsRowShown="0">
+  <autoFilter ref="A1:E63" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="date" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="test" dataDxfId="3"/>
@@ -918,10 +918,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E62"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+      <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1917,6 +1917,23 @@
         <v>3109</v>
       </c>
     </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>43964</v>
+      </c>
+      <c r="B63" s="2">
+        <v>33332</v>
+      </c>
+      <c r="C63" s="2">
+        <v>1639</v>
+      </c>
+      <c r="D63" s="2">
+        <v>58</v>
+      </c>
+      <c r="E63" s="2">
+        <v>2826</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
14 Mayıs 2020 verileri eklendi
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\github\covid19-turkey\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1572F037-7A9E-4F37-AAD2-46425ABB51A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CAD0FE5-A281-406D-9AEA-B92D6F61C20E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -608,8 +608,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:E63" totalsRowShown="0">
-  <autoFilter ref="A1:E63" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:E64" totalsRowShown="0">
+  <autoFilter ref="A1:E64" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="date" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="test" dataDxfId="3"/>
@@ -918,7 +918,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E63"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
       <selection activeCell="E63" sqref="E63"/>
@@ -1934,6 +1934,23 @@
         <v>2826</v>
       </c>
     </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>43965</v>
+      </c>
+      <c r="B64" s="2">
+        <v>34821</v>
+      </c>
+      <c r="C64" s="2">
+        <v>1635</v>
+      </c>
+      <c r="D64" s="2">
+        <v>55</v>
+      </c>
+      <c r="E64" s="2">
+        <v>2315</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
15 Mayıs 2020 verileri eklendi
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\github\covid19-turkey\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mehmet\Desktop\github\covid19-turkey\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CAD0FE5-A281-406D-9AEA-B92D6F61C20E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -534,48 +533,48 @@
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="%20 - Vurgu1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="%20 - Vurgu2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="%20 - Vurgu3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="%20 - Vurgu4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="%20 - Vurgu5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="%20 - Vurgu6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="%40 - Vurgu1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="%40 - Vurgu2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="%40 - Vurgu3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="%40 - Vurgu4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="%40 - Vurgu5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="%40 - Vurgu6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="%60 - Vurgu1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="%60 - Vurgu2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="%60 - Vurgu3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="%60 - Vurgu4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="%60 - Vurgu5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="%60 - Vurgu6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Açıklama Metni" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Ana Başlık" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Bağlı Hücre" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Başlık 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Başlık 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Başlık 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Başlık 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Çıkış" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Giriş" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Hesaplama" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="İşaretli Hücre" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="İyi" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Kötü" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Not" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Nötr" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Toplam" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Uyarı Metni" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Vurgu1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Vurgu2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Vurgu3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Vurgu4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Vurgu5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Vurgu6" xfId="38" builtinId="49" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
@@ -608,14 +607,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:E64" totalsRowShown="0">
-  <autoFilter ref="A1:E64" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:E65" totalsRowShown="0">
+  <autoFilter ref="A1:E65"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="date" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="test" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="case" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="death" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="recovered" dataDxfId="0"/>
+    <tableColumn id="1" name="date" dataDxfId="4"/>
+    <tableColumn id="2" name="test" dataDxfId="3"/>
+    <tableColumn id="3" name="case" dataDxfId="2"/>
+    <tableColumn id="4" name="death" dataDxfId="1"/>
+    <tableColumn id="5" name="recovered" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -917,11 +916,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E64"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="E63" sqref="E63"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1951,6 +1950,23 @@
         <v>2315</v>
       </c>
     </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>43966</v>
+      </c>
+      <c r="B65" s="2">
+        <v>38565</v>
+      </c>
+      <c r="C65" s="2">
+        <v>1708</v>
+      </c>
+      <c r="D65" s="2">
+        <v>48</v>
+      </c>
+      <c r="E65" s="2">
+        <v>2103</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
16 Mayıs 2020 verileri eklendi
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -607,8 +607,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:E65" totalsRowShown="0">
-  <autoFilter ref="A1:E65"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:E66" totalsRowShown="0">
+  <autoFilter ref="A1:E66"/>
   <tableColumns count="5">
     <tableColumn id="1" name="date" dataDxfId="4"/>
     <tableColumn id="2" name="test" dataDxfId="3"/>
@@ -917,7 +917,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E65"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
       <selection activeCell="E65" sqref="E65"/>
@@ -1967,6 +1967,23 @@
         <v>2103</v>
       </c>
     </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>43967</v>
+      </c>
+      <c r="B66" s="2">
+        <v>42236</v>
+      </c>
+      <c r="C66" s="2">
+        <v>1610</v>
+      </c>
+      <c r="D66" s="2">
+        <v>41</v>
+      </c>
+      <c r="E66" s="2">
+        <v>2004</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
17 Mayıs 2020 verileri eklendi
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -607,8 +607,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:E66" totalsRowShown="0">
-  <autoFilter ref="A1:E66"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:E67" totalsRowShown="0">
+  <autoFilter ref="A1:E67"/>
   <tableColumns count="5">
     <tableColumn id="1" name="date" dataDxfId="4"/>
     <tableColumn id="2" name="test" dataDxfId="3"/>
@@ -917,10 +917,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E66"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65"/>
+      <selection activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1984,6 +1984,23 @@
         <v>2004</v>
       </c>
     </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>43968</v>
+      </c>
+      <c r="B67" s="2">
+        <v>35369</v>
+      </c>
+      <c r="C67" s="2">
+        <v>1368</v>
+      </c>
+      <c r="D67" s="2">
+        <v>44</v>
+      </c>
+      <c r="E67" s="2">
+        <v>1825</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
18 Mayıs 2020 verileri eklendi
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mehmet\Desktop\github\covid19-turkey\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\github\covid19-turkey\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8618558-A6C8-41EE-82A0-9D9FCDD3709A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -533,48 +534,48 @@
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="%20 - Vurgu1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="%20 - Vurgu2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="%20 - Vurgu3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="%20 - Vurgu4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="%20 - Vurgu5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="%20 - Vurgu6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="%40 - Vurgu1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="%40 - Vurgu2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="%40 - Vurgu3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="%40 - Vurgu4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="%40 - Vurgu5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="%40 - Vurgu6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="%60 - Vurgu1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="%60 - Vurgu2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="%60 - Vurgu3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="%60 - Vurgu4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="%60 - Vurgu5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="%60 - Vurgu6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Açıklama Metni" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Ana Başlık" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Bağlı Hücre" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Başlık 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Başlık 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Başlık 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Başlık 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Çıkış" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Giriş" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Hesaplama" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="İşaretli Hücre" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="İyi" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Kötü" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Not" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Nötr" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Toplam" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Uyarı Metni" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Vurgu1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Vurgu2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Vurgu3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Vurgu4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Vurgu5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Vurgu6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
@@ -607,14 +608,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:E67" totalsRowShown="0">
-  <autoFilter ref="A1:E67"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:E68" totalsRowShown="0">
+  <autoFilter ref="A1:E68" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="date" dataDxfId="4"/>
-    <tableColumn id="2" name="test" dataDxfId="3"/>
-    <tableColumn id="3" name="case" dataDxfId="2"/>
-    <tableColumn id="4" name="death" dataDxfId="1"/>
-    <tableColumn id="5" name="recovered" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="date" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="test" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="case" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="death" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="recovered" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -916,22 +917,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E67"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66"/>
+      <selection activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="15" style="2" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="2"/>
-    <col min="5" max="5" width="10.7109375" style="2" customWidth="1"/>
+    <col min="3" max="4" width="9.109375" style="2"/>
+    <col min="5" max="5" width="10.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -948,7 +949,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43903</v>
       </c>
@@ -956,7 +957,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43904</v>
       </c>
@@ -964,7 +965,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>43905</v>
       </c>
@@ -972,7 +973,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>43906</v>
       </c>
@@ -980,7 +981,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>43907</v>
       </c>
@@ -991,7 +992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>43908</v>
       </c>
@@ -1002,7 +1003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>43909</v>
       </c>
@@ -1016,7 +1017,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>43910</v>
       </c>
@@ -1030,7 +1031,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>43911</v>
       </c>
@@ -1044,7 +1045,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>43912</v>
       </c>
@@ -1058,7 +1059,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>43913</v>
       </c>
@@ -1072,7 +1073,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>43914</v>
       </c>
@@ -1089,7 +1090,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>43915</v>
       </c>
@@ -1103,7 +1104,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>43916</v>
       </c>
@@ -1117,7 +1118,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>43917</v>
       </c>
@@ -1134,7 +1135,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>43918</v>
       </c>
@@ -1151,7 +1152,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>43919</v>
       </c>
@@ -1168,7 +1169,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>43920</v>
       </c>
@@ -1185,7 +1186,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>43921</v>
       </c>
@@ -1202,7 +1203,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>43922</v>
       </c>
@@ -1219,7 +1220,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>43923</v>
       </c>
@@ -1236,7 +1237,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>43924</v>
       </c>
@@ -1253,7 +1254,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>43925</v>
       </c>
@@ -1270,7 +1271,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>43926</v>
       </c>
@@ -1287,7 +1288,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>43927</v>
       </c>
@@ -1304,7 +1305,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>43928</v>
       </c>
@@ -1321,7 +1322,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>43929</v>
       </c>
@@ -1338,7 +1339,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>43930</v>
       </c>
@@ -1355,7 +1356,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>43931</v>
       </c>
@@ -1372,7 +1373,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>43932</v>
       </c>
@@ -1389,7 +1390,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>43933</v>
       </c>
@@ -1406,7 +1407,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>43934</v>
       </c>
@@ -1423,7 +1424,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>43935</v>
       </c>
@@ -1440,7 +1441,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>43936</v>
       </c>
@@ -1457,7 +1458,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>43937</v>
       </c>
@@ -1474,7 +1475,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>43938</v>
       </c>
@@ -1491,7 +1492,7 @@
         <v>1542</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>43939</v>
       </c>
@@ -1508,7 +1509,7 @@
         <v>1822</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>43940</v>
       </c>
@@ -1525,7 +1526,7 @@
         <v>1523</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>43941</v>
       </c>
@@ -1542,7 +1543,7 @@
         <v>1454</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>43942</v>
       </c>
@@ -1559,7 +1560,7 @@
         <v>1488</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>43943</v>
       </c>
@@ -1576,7 +1577,7 @@
         <v>1559</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>43944</v>
       </c>
@@ -1593,7 +1594,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>43945</v>
       </c>
@@ -1610,7 +1611,7 @@
         <v>3246</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>43946</v>
       </c>
@@ -1627,7 +1628,7 @@
         <v>3845</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>43947</v>
       </c>
@@ -1644,7 +1645,7 @@
         <v>3558</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>43948</v>
       </c>
@@ -1661,7 +1662,7 @@
         <v>4651</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>43949</v>
       </c>
@@ -1678,7 +1679,7 @@
         <v>5018</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>43950</v>
       </c>
@@ -1695,7 +1696,7 @@
         <v>5231</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>43951</v>
       </c>
@@ -1712,7 +1713,7 @@
         <v>4846</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>43952</v>
       </c>
@@ -1729,7 +1730,7 @@
         <v>4922</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>43953</v>
       </c>
@@ -1746,7 +1747,7 @@
         <v>4451</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>43954</v>
       </c>
@@ -1763,7 +1764,7 @@
         <v>4892</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>43955</v>
       </c>
@@ -1780,7 +1781,7 @@
         <v>5015</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>43956</v>
       </c>
@@ -1797,7 +1798,7 @@
         <v>5119</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>43957</v>
       </c>
@@ -1814,7 +1815,7 @@
         <v>4917</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>43958</v>
       </c>
@@ -1831,7 +1832,7 @@
         <v>4782</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>43959</v>
       </c>
@@ -1848,7 +1849,7 @@
         <v>3412</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>43960</v>
       </c>
@@ -1865,7 +1866,7 @@
         <v>3084</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>43961</v>
       </c>
@@ -1882,7 +1883,7 @@
         <v>3211</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>43962</v>
       </c>
@@ -1899,7 +1900,7 @@
         <v>3089</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>43963</v>
       </c>
@@ -1916,7 +1917,7 @@
         <v>3109</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>43964</v>
       </c>
@@ -1933,7 +1934,7 @@
         <v>2826</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>43965</v>
       </c>
@@ -1950,7 +1951,7 @@
         <v>2315</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>43966</v>
       </c>
@@ -1967,7 +1968,7 @@
         <v>2103</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>43967</v>
       </c>
@@ -1984,7 +1985,7 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>43968</v>
       </c>
@@ -1999,6 +2000,23 @@
       </c>
       <c r="E67" s="2">
         <v>1825</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" s="1">
+        <v>43969</v>
+      </c>
+      <c r="B68" s="2">
+        <v>25141</v>
+      </c>
+      <c r="C68" s="2">
+        <v>1158</v>
+      </c>
+      <c r="D68" s="2">
+        <v>31</v>
+      </c>
+      <c r="E68" s="2">
+        <v>1615</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
19 Mayıs 2020 verileri eklendi
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\github\covid19-turkey\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8618558-A6C8-41EE-82A0-9D9FCDD3709A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72E4102-FD38-4EF5-9E69-F49CF0D9D07D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>test</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t>date</t>
+  </si>
+  <si>
+    <t>o</t>
   </si>
 </sst>
 </file>
@@ -608,8 +611,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:E68" totalsRowShown="0">
-  <autoFilter ref="A1:E68" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:E69" totalsRowShown="0">
+  <autoFilter ref="A1:E69" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="date" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="test" dataDxfId="3"/>
@@ -918,21 +921,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E68"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="E67" sqref="E67"/>
+      <selection activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="15" style="2" customWidth="1"/>
-    <col min="3" max="4" width="9.109375" style="2"/>
-    <col min="5" max="5" width="10.6640625" style="2" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="2"/>
+    <col min="5" max="5" width="10.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -949,7 +952,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43903</v>
       </c>
@@ -957,7 +960,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43904</v>
       </c>
@@ -965,7 +968,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43905</v>
       </c>
@@ -973,7 +976,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43906</v>
       </c>
@@ -981,7 +984,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43907</v>
       </c>
@@ -992,7 +995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43908</v>
       </c>
@@ -1003,7 +1006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43909</v>
       </c>
@@ -1017,7 +1020,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43910</v>
       </c>
@@ -1031,7 +1034,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43911</v>
       </c>
@@ -1045,7 +1048,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43912</v>
       </c>
@@ -1059,7 +1062,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43913</v>
       </c>
@@ -1073,7 +1076,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43914</v>
       </c>
@@ -1090,7 +1093,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43915</v>
       </c>
@@ -1104,7 +1107,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43916</v>
       </c>
@@ -1118,7 +1121,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43917</v>
       </c>
@@ -1135,7 +1138,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43918</v>
       </c>
@@ -1152,7 +1155,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>43919</v>
       </c>
@@ -1169,7 +1172,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>43920</v>
       </c>
@@ -1186,7 +1189,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>43921</v>
       </c>
@@ -1203,7 +1206,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>43922</v>
       </c>
@@ -1220,7 +1223,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43923</v>
       </c>
@@ -1237,7 +1240,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>43924</v>
       </c>
@@ -1254,7 +1257,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>43925</v>
       </c>
@@ -1271,7 +1274,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>43926</v>
       </c>
@@ -1288,7 +1291,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>43927</v>
       </c>
@@ -1305,7 +1308,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>43928</v>
       </c>
@@ -1322,7 +1325,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>43929</v>
       </c>
@@ -1339,7 +1342,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>43930</v>
       </c>
@@ -1356,7 +1359,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>43931</v>
       </c>
@@ -1373,7 +1376,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>43932</v>
       </c>
@@ -1390,7 +1393,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>43933</v>
       </c>
@@ -1407,7 +1410,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>43934</v>
       </c>
@@ -1424,7 +1427,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>43935</v>
       </c>
@@ -1441,7 +1444,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>43936</v>
       </c>
@@ -1458,7 +1461,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>43937</v>
       </c>
@@ -1475,7 +1478,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>43938</v>
       </c>
@@ -1492,7 +1495,7 @@
         <v>1542</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>43939</v>
       </c>
@@ -1509,7 +1512,7 @@
         <v>1822</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>43940</v>
       </c>
@@ -1526,7 +1529,7 @@
         <v>1523</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>43941</v>
       </c>
@@ -1543,7 +1546,7 @@
         <v>1454</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>43942</v>
       </c>
@@ -1560,7 +1563,7 @@
         <v>1488</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>43943</v>
       </c>
@@ -1577,7 +1580,7 @@
         <v>1559</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>43944</v>
       </c>
@@ -1594,7 +1597,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43945</v>
       </c>
@@ -1611,7 +1614,7 @@
         <v>3246</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43946</v>
       </c>
@@ -1628,7 +1631,7 @@
         <v>3845</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>43947</v>
       </c>
@@ -1645,7 +1648,7 @@
         <v>3558</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>43948</v>
       </c>
@@ -1662,7 +1665,7 @@
         <v>4651</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>43949</v>
       </c>
@@ -1679,7 +1682,7 @@
         <v>5018</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>43950</v>
       </c>
@@ -1696,7 +1699,7 @@
         <v>5231</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>43951</v>
       </c>
@@ -1713,7 +1716,7 @@
         <v>4846</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>43952</v>
       </c>
@@ -1730,7 +1733,7 @@
         <v>4922</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>43953</v>
       </c>
@@ -1747,7 +1750,7 @@
         <v>4451</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>43954</v>
       </c>
@@ -1764,7 +1767,7 @@
         <v>4892</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>43955</v>
       </c>
@@ -1781,7 +1784,7 @@
         <v>5015</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>43956</v>
       </c>
@@ -1798,7 +1801,7 @@
         <v>5119</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>43957</v>
       </c>
@@ -1815,7 +1818,7 @@
         <v>4917</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>43958</v>
       </c>
@@ -1832,7 +1835,7 @@
         <v>4782</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>43959</v>
       </c>
@@ -1849,7 +1852,7 @@
         <v>3412</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>43960</v>
       </c>
@@ -1866,7 +1869,7 @@
         <v>3084</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>43961</v>
       </c>
@@ -1883,7 +1886,7 @@
         <v>3211</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>43962</v>
       </c>
@@ -1900,7 +1903,7 @@
         <v>3089</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>43963</v>
       </c>
@@ -1917,7 +1920,7 @@
         <v>3109</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>43964</v>
       </c>
@@ -1934,7 +1937,7 @@
         <v>2826</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>43965</v>
       </c>
@@ -1951,7 +1954,7 @@
         <v>2315</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>43966</v>
       </c>
@@ -1968,7 +1971,7 @@
         <v>2103</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>43967</v>
       </c>
@@ -1985,7 +1988,7 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>43968</v>
       </c>
@@ -1998,11 +2001,11 @@
       <c r="D67" s="2">
         <v>44</v>
       </c>
-      <c r="E67" s="2">
-        <v>1825</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E67" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>43969</v>
       </c>
@@ -2017,6 +2020,23 @@
       </c>
       <c r="E68" s="2">
         <v>1615</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>43970</v>
+      </c>
+      <c r="B69" s="2">
+        <v>25382</v>
+      </c>
+      <c r="C69" s="2">
+        <v>1022</v>
+      </c>
+      <c r="D69" s="2">
+        <v>28</v>
+      </c>
+      <c r="E69" s="2">
+        <v>1318</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
20 Mayıs 2020 verileri eklendi
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\github\covid19-turkey\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72E4102-FD38-4EF5-9E69-F49CF0D9D07D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1FC9F09-0ABC-4AB7-9380-0D1E6FE022C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>test</t>
   </si>
@@ -35,9 +35,6 @@
   </si>
   <si>
     <t>date</t>
-  </si>
-  <si>
-    <t>o</t>
   </si>
 </sst>
 </file>
@@ -611,8 +608,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:E69" totalsRowShown="0">
-  <autoFilter ref="A1:E69" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:E70" totalsRowShown="0">
+  <autoFilter ref="A1:E70" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="date" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="test" dataDxfId="3"/>
@@ -921,7 +918,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
       <selection activeCell="E68" sqref="E68"/>
@@ -2001,8 +1998,8 @@
       <c r="D67" s="2">
         <v>44</v>
       </c>
-      <c r="E67" s="2" t="s">
-        <v>5</v>
+      <c r="E67" s="2">
+        <v>1825</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -2037,6 +2034,23 @@
       </c>
       <c r="E69" s="2">
         <v>1318</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>43971</v>
+      </c>
+      <c r="B70" s="2">
+        <v>20838</v>
+      </c>
+      <c r="C70" s="2">
+        <v>972</v>
+      </c>
+      <c r="D70" s="2">
+        <v>23</v>
+      </c>
+      <c r="E70" s="2">
+        <v>1092</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
21 Mayıs 2020 verileri eklendi.
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\github\covid19-turkey\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11010269-67AC-408C-A6A1-3FA868B3AA17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2486B8CE-BEF1-4C47-A0A4-5210CF0802D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -618,8 +618,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:E70" totalsRowShown="0">
-  <autoFilter ref="A1:E70" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:E71" totalsRowShown="0">
+  <autoFilter ref="A1:E71" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="date" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="test" dataDxfId="3"/>
@@ -928,10 +928,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2081,6 +2081,23 @@
         <v>1092</v>
       </c>
     </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>43972</v>
+      </c>
+      <c r="B71" s="2">
+        <v>33633</v>
+      </c>
+      <c r="C71" s="2">
+        <v>961</v>
+      </c>
+      <c r="D71" s="2">
+        <v>27</v>
+      </c>
+      <c r="E71" s="2">
+        <v>1003</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
22 Mayıs 2020 verileri eklendi
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\github\covid19-turkey\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2486B8CE-BEF1-4C47-A0A4-5210CF0802D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4A2362-F5F8-4CE9-A21C-5AFFE33E0F28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -618,8 +618,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:E71" totalsRowShown="0">
-  <autoFilter ref="A1:E71" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:E72" totalsRowShown="0">
+  <autoFilter ref="A1:E72" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="date" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="test" dataDxfId="3"/>
@@ -928,10 +928,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="E70" sqref="E70"/>
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2098,6 +2098,23 @@
         <v>1003</v>
       </c>
     </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>43973</v>
+      </c>
+      <c r="B72" s="2">
+        <v>37507</v>
+      </c>
+      <c r="C72" s="2">
+        <v>952</v>
+      </c>
+      <c r="D72" s="2">
+        <v>27</v>
+      </c>
+      <c r="E72" s="2">
+        <v>1121</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
23 mayıs verileri eklendi
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\github\covid19-turkey\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4A2362-F5F8-4CE9-A21C-5AFFE33E0F28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3214A185-C09F-447B-AFA3-C2664AB2DEB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -618,8 +618,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:E72" totalsRowShown="0">
-  <autoFilter ref="A1:E72" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:E73" totalsRowShown="0">
+  <autoFilter ref="A1:E73" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="date" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="test" dataDxfId="3"/>
@@ -928,10 +928,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2115,6 +2115,23 @@
         <v>1121</v>
       </c>
     </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>43974</v>
+      </c>
+      <c r="B73" s="2">
+        <v>40178</v>
+      </c>
+      <c r="C73" s="2">
+        <v>1186</v>
+      </c>
+      <c r="D73" s="2">
+        <v>32</v>
+      </c>
+      <c r="E73" s="2">
+        <v>1491</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
24 mayıs verileri eklendi.
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\github\covid19-turkey\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mehmet\Desktop\github\covid19-turkey\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3214A185-C09F-447B-AFA3-C2664AB2DEB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -50,7 +49,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -544,48 +543,48 @@
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="%20 - Vurgu1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="%20 - Vurgu2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="%20 - Vurgu3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="%20 - Vurgu4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="%20 - Vurgu5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="%20 - Vurgu6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="%40 - Vurgu1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="%40 - Vurgu2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="%40 - Vurgu3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="%40 - Vurgu4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="%40 - Vurgu5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="%40 - Vurgu6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="%60 - Vurgu1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="%60 - Vurgu2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="%60 - Vurgu3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="%60 - Vurgu4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="%60 - Vurgu5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="%60 - Vurgu6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Açıklama Metni" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Ana Başlık" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Bağlı Hücre" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Başlık 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Başlık 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Başlık 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Başlık 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Çıkış" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Giriş" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Hesaplama" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="İşaretli Hücre" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="İyi" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Kötü" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Not" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Nötr" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Toplam" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Uyarı Metni" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Vurgu1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Vurgu2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Vurgu3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Vurgu4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Vurgu5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Vurgu6" xfId="38" builtinId="49" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
@@ -618,14 +617,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:E73" totalsRowShown="0">
-  <autoFilter ref="A1:E73" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:E74" totalsRowShown="0">
+  <autoFilter ref="A1:E74"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="date" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="test" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="case" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="death" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="recovered" dataDxfId="0"/>
+    <tableColumn id="1" name="date" dataDxfId="4"/>
+    <tableColumn id="2" name="test" dataDxfId="3"/>
+    <tableColumn id="3" name="case" dataDxfId="2"/>
+    <tableColumn id="4" name="death" dataDxfId="1"/>
+    <tableColumn id="5" name="recovered" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -927,11 +926,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E73"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E74"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C73" sqref="C73"/>
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2132,6 +2131,23 @@
         <v>1491</v>
       </c>
     </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>43975</v>
+      </c>
+      <c r="B74" s="2">
+        <v>24589</v>
+      </c>
+      <c r="C74" s="2">
+        <v>1141</v>
+      </c>
+      <c r="D74" s="2">
+        <v>32</v>
+      </c>
+      <c r="E74" s="2">
+        <v>1092</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
25 Mayıs verileri eklendi
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -617,8 +617,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:E74" totalsRowShown="0">
-  <autoFilter ref="A1:E74"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:E75" totalsRowShown="0">
+  <autoFilter ref="A1:E75"/>
   <tableColumns count="5">
     <tableColumn id="1" name="date" dataDxfId="4"/>
     <tableColumn id="2" name="test" dataDxfId="3"/>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E74"/>
+  <dimension ref="A1:E75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="E73" sqref="E73"/>
+      <selection activeCell="E74" sqref="E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2148,6 +2148,23 @@
         <v>1092</v>
       </c>
     </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>43976</v>
+      </c>
+      <c r="B75" s="2">
+        <v>21492</v>
+      </c>
+      <c r="C75" s="2">
+        <v>987</v>
+      </c>
+      <c r="D75" s="2">
+        <v>29</v>
+      </c>
+      <c r="E75" s="2">
+        <v>1321</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
26 Mayıs verileri eklendi
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1,30 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mehmet\Desktop\github\covid19-turkey\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\github\covid19-turkey\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A331E6E-D1D4-4442-A2C3-353DF868D2A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -49,7 +40,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -543,48 +534,48 @@
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="%20 - Vurgu1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="%20 - Vurgu2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="%20 - Vurgu3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="%20 - Vurgu4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="%20 - Vurgu5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="%20 - Vurgu6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="%40 - Vurgu1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="%40 - Vurgu2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="%40 - Vurgu3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="%40 - Vurgu4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="%40 - Vurgu5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="%40 - Vurgu6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="%60 - Vurgu1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="%60 - Vurgu2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="%60 - Vurgu3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="%60 - Vurgu4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="%60 - Vurgu5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="%60 - Vurgu6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Açıklama Metni" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Ana Başlık" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Bağlı Hücre" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Başlık 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Başlık 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Başlık 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Başlık 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Çıkış" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Giriş" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Hesaplama" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="İşaretli Hücre" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="İyi" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Kötü" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Not" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Nötr" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Toplam" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Uyarı Metni" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Vurgu1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Vurgu2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Vurgu3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Vurgu4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Vurgu5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Vurgu6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
@@ -617,14 +608,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:E75" totalsRowShown="0">
-  <autoFilter ref="A1:E75"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:E76" totalsRowShown="0">
+  <autoFilter ref="A1:E76" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="date" dataDxfId="4"/>
-    <tableColumn id="2" name="test" dataDxfId="3"/>
-    <tableColumn id="3" name="case" dataDxfId="2"/>
-    <tableColumn id="4" name="death" dataDxfId="1"/>
-    <tableColumn id="5" name="recovered" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="date" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="test" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="case" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="death" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="recovered" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -926,11 +917,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E76"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="E74" sqref="E74"/>
+      <selection activeCell="B77" sqref="B77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2165,6 +2156,23 @@
         <v>1321</v>
       </c>
     </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>43977</v>
+      </c>
+      <c r="B76" s="2">
+        <v>19853</v>
+      </c>
+      <c r="C76" s="2">
+        <v>948</v>
+      </c>
+      <c r="D76" s="2">
+        <v>28</v>
+      </c>
+      <c r="E76" s="2">
+        <v>1492</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
27 Mayıs verileri eklendi
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\github\covid19-turkey\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A331E6E-D1D4-4442-A2C3-353DF868D2A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1FF20B-9D88-4E9E-B64E-A665B196AD1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -608,8 +608,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:E76" totalsRowShown="0">
-  <autoFilter ref="A1:E76" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:E77" totalsRowShown="0">
+  <autoFilter ref="A1:E77" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="date" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="test" dataDxfId="3"/>
@@ -918,10 +918,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E76"/>
+  <dimension ref="A1:E77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B77" sqref="B77"/>
+      <selection activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2173,6 +2173,23 @@
         <v>1492</v>
       </c>
     </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>43978</v>
+      </c>
+      <c r="B77" s="2">
+        <v>21043</v>
+      </c>
+      <c r="C77" s="2">
+        <v>1035</v>
+      </c>
+      <c r="D77" s="2">
+        <v>34</v>
+      </c>
+      <c r="E77" s="2">
+        <v>1286</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
28 Mayıs verileri eklendi
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\github\covid19-turkey\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1FF20B-9D88-4E9E-B64E-A665B196AD1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2FB09D5-DD24-43AE-9160-74E9EBB85ED3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -608,8 +608,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:E77" totalsRowShown="0">
-  <autoFilter ref="A1:E77" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:E78" totalsRowShown="0">
+  <autoFilter ref="A1:E78" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="date" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="test" dataDxfId="3"/>
@@ -918,10 +918,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E77"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78"/>
+      <selection activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2190,6 +2190,23 @@
         <v>1286</v>
       </c>
     </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>43979</v>
+      </c>
+      <c r="B78" s="2">
+        <v>33559</v>
+      </c>
+      <c r="C78" s="2">
+        <v>1182</v>
+      </c>
+      <c r="D78" s="2">
+        <v>30</v>
+      </c>
+      <c r="E78" s="2">
+        <v>1576</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
29 Mayıs verileri eklendi.
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\github\covid19-turkey\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1FF20B-9D88-4E9E-B64E-A665B196AD1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2FB09D5-DD24-43AE-9160-74E9EBB85ED3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -608,8 +608,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:E77" totalsRowShown="0">
-  <autoFilter ref="A1:E77" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:E78" totalsRowShown="0">
+  <autoFilter ref="A1:E78" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="date" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="test" dataDxfId="3"/>
@@ -918,10 +918,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E77"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78"/>
+      <selection activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2190,6 +2190,23 @@
         <v>1286</v>
       </c>
     </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>43979</v>
+      </c>
+      <c r="B78" s="2">
+        <v>33559</v>
+      </c>
+      <c r="C78" s="2">
+        <v>1182</v>
+      </c>
+      <c r="D78" s="2">
+        <v>30</v>
+      </c>
+      <c r="E78" s="2">
+        <v>1576</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
29 ve 30 Mayıs verileri eklendi
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\github\covid19-turkey\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2FB09D5-DD24-43AE-9160-74E9EBB85ED3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B70449DC-45A2-47D0-906E-6F0DD0267EF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -608,8 +608,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:E78" totalsRowShown="0">
-  <autoFilter ref="A1:E78" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:E80" totalsRowShown="0">
+  <autoFilter ref="A1:E80" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="date" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="test" dataDxfId="3"/>
@@ -918,10 +918,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E78"/>
+  <dimension ref="A1:E80"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="E77" sqref="E77"/>
+      <selection activeCell="E80" sqref="E80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2207,6 +2207,40 @@
         <v>1576</v>
       </c>
     </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>43980</v>
+      </c>
+      <c r="B79" s="2">
+        <v>36155</v>
+      </c>
+      <c r="C79" s="2">
+        <v>1141</v>
+      </c>
+      <c r="D79" s="2">
+        <v>28</v>
+      </c>
+      <c r="E79" s="2">
+        <v>1594</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>43981</v>
+      </c>
+      <c r="B80" s="2">
+        <v>39230</v>
+      </c>
+      <c r="C80" s="2">
+        <v>983</v>
+      </c>
+      <c r="D80" s="2">
+        <v>26</v>
+      </c>
+      <c r="E80" s="2">
+        <v>1021</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
31 Mayıs verileri eklendi
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\github\covid19-turkey\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B70449DC-45A2-47D0-906E-6F0DD0267EF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F544A80-01A2-42C6-9F8A-82E384FB4B15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -608,8 +608,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:E80" totalsRowShown="0">
-  <autoFilter ref="A1:E80" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:E81" totalsRowShown="0">
+  <autoFilter ref="A1:E81" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="date" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="test" dataDxfId="3"/>
@@ -918,7 +918,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E80"/>
+  <dimension ref="A1:E81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
       <selection activeCell="E80" sqref="E80"/>
@@ -2241,6 +2241,23 @@
         <v>1021</v>
       </c>
     </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>43982</v>
+      </c>
+      <c r="B81" s="2">
+        <v>35600</v>
+      </c>
+      <c r="C81" s="2">
+        <v>839</v>
+      </c>
+      <c r="D81" s="2">
+        <v>25</v>
+      </c>
+      <c r="E81" s="2">
+        <v>989</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>